<commit_message>
upd: ExSkins colors / ExRoles Impostor roles
</commit_message>
<xml_diff>
--- a/ExtremeSkinsTransData.xlsx
+++ b/ExtremeSkinsTransData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GIT\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE4DB4-A0A5-47A8-9A54-7A67FEC8EED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D845BDE9-F8E2-4107-A53C-FA621A35B62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="510" windowWidth="25035" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="171">
   <si>
     <t>English</t>
   </si>
@@ -642,6 +642,86 @@
   </si>
   <si>
     <t>kigi</t>
+  </si>
+  <si>
+    <t>Medium Violet Red</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Medium Purple</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pale Cyan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>White-Pink</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Thin Purple</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sienna</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Light Avocado</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Light Iwai-cha</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Diard Red</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Chaos</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Inverted</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Odd Green</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tiger</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kigi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dark Sepia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Diard Green</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Diard Blue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Creator mode Enabled</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disabling Creator mode on restart</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enabling Creator mode on restart</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -994,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB33A825-820B-4CCD-9FAD-3D139F562B99}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1146,6 +1226,9 @@
       <c r="A10" t="s">
         <v>117</v>
       </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
       <c r="M10" t="s">
         <v>122</v>
       </c>
@@ -1154,6 +1237,9 @@
       <c r="A11" t="s">
         <v>118</v>
       </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
       <c r="M11" t="s">
         <v>121</v>
       </c>
@@ -1161,6 +1247,9 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>170</v>
       </c>
       <c r="M12" t="s">
         <v>120</v>
@@ -1177,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1271,6 +1360,9 @@
       <c r="A4" t="s">
         <v>29</v>
       </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
       <c r="M4" t="s">
         <v>31</v>
       </c>
@@ -1282,6 +1374,9 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
       <c r="M5" t="s">
         <v>33</v>
       </c>
@@ -1461,6 +1556,9 @@
       <c r="A18" t="s">
         <v>58</v>
       </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
       <c r="M18" t="s">
         <v>59</v>
       </c>
@@ -1514,6 +1612,9 @@
       <c r="A22" t="s">
         <v>133</v>
       </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
       <c r="M22" t="s">
         <v>134</v>
       </c>
@@ -1522,6 +1623,9 @@
       <c r="A23" t="s">
         <v>135</v>
       </c>
+      <c r="B23" t="s">
+        <v>154</v>
+      </c>
       <c r="M23" t="s">
         <v>136</v>
       </c>
@@ -1530,6 +1634,9 @@
       <c r="A24" t="s">
         <v>137</v>
       </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
       <c r="M24" t="s">
         <v>138</v>
       </c>
@@ -1538,6 +1645,9 @@
       <c r="A25" t="s">
         <v>139</v>
       </c>
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
       <c r="M25" t="s">
         <v>140</v>
       </c>
@@ -1546,6 +1656,9 @@
       <c r="A26" t="s">
         <v>141</v>
       </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
       <c r="M26" t="s">
         <v>142</v>
       </c>
@@ -1554,6 +1667,9 @@
       <c r="A27" t="s">
         <v>143</v>
       </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
       <c r="M27" t="s">
         <v>144</v>
       </c>
@@ -1562,6 +1678,9 @@
       <c r="A28" t="s">
         <v>130</v>
       </c>
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
       <c r="M28" t="s">
         <v>127</v>
       </c>
@@ -1570,6 +1689,9 @@
       <c r="A29" t="s">
         <v>131</v>
       </c>
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
       <c r="M29" t="s">
         <v>128</v>
       </c>
@@ -1578,6 +1700,9 @@
       <c r="A30" t="s">
         <v>132</v>
       </c>
+      <c r="B30" t="s">
+        <v>167</v>
+      </c>
       <c r="M30" t="s">
         <v>129</v>
       </c>
@@ -1586,6 +1711,9 @@
       <c r="A31" t="s">
         <v>123</v>
       </c>
+      <c r="B31" t="s">
+        <v>160</v>
+      </c>
       <c r="M31" t="s">
         <v>124</v>
       </c>
@@ -1594,6 +1722,9 @@
       <c r="A32" t="s">
         <v>125</v>
       </c>
+      <c r="B32" t="s">
+        <v>161</v>
+      </c>
       <c r="M32" t="s">
         <v>126</v>
       </c>
@@ -1602,6 +1733,9 @@
       <c r="A33" t="s">
         <v>145</v>
       </c>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
       <c r="M33" t="s">
         <v>146</v>
       </c>
@@ -1610,6 +1744,9 @@
       <c r="A34" t="s">
         <v>147</v>
       </c>
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
       <c r="M34" t="s">
         <v>148</v>
       </c>
@@ -1617,6 +1754,9 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
       </c>
       <c r="M35" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
feat : new color
</commit_message>
<xml_diff>
--- a/ExtremeSkinsTransData.xlsx
+++ b/ExtremeSkinsTransData.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileSharing readOnlyRecommended="0" userName="yukieiji"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14617" windowHeight="8160" activeTab="1"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="14610" windowHeight="8160" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="System" sheetId="6" r:id="rId1"/>
-    <sheet name="Color" sheetId="5" r:id="rId2"/>
+    <sheet name="System" sheetId="1" r:id="rId4"/>
+    <sheet name="Color" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr/>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:revision xmlns:pm="smNativeData" day="1753718275" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1753718275" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1753718275" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1753718275"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="196">
   <si>
     <t>English</t>
   </si>
@@ -579,179 +588,360 @@
   </si>
   <si>
     <t>基吉色</t>
+  </si>
+  <si>
+    <t>whisky</t>
+  </si>
+  <si>
+    <t>ウィスキー</t>
+  </si>
+  <si>
+    <t>geranium</t>
+  </si>
+  <si>
+    <t>ジェラニョム</t>
+  </si>
+  <si>
+    <t>fuchsia</t>
+  </si>
+  <si>
+    <t>フクシャ</t>
+  </si>
+  <si>
+    <t>safeBlue</t>
+  </si>
+  <si>
+    <t>セーフブルー</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="13">
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;¥&quot;;\-#,##0\ &quot;¥&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;¥&quot;;[Red]\-#,##0\ &quot;¥&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;¥&quot;;\-#,##0.00\ &quot;¥&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;¥&quot;;[Red]\-#,##0.00\ &quot;¥&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;¥&quot;_-;\-* #,##0\ &quot;¥&quot;_-;_-* &quot;-&quot;\ &quot;¥&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _¥_-;\-* #,##0\ _¥_-;_-* &quot;-&quot;\ _¥_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;¥&quot;_-;\-* #,##0.00\ &quot;¥&quot;_-;_-* &quot;-&quot;??\ &quot;¥&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _¥_-;\-* #,##0.00\ _¥_-;_-* &quot;-&quot;??\ _¥_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="9" formatCode="0%"/>
   </numFmts>
   <fonts count="21">
     <font>
+      <name val="等线"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <color rgb="FF3F3F76"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="3F3F76" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <color rgb="FF9C0006"/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="9C0006" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="FFFFFF" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <color rgb="FF0000FF"/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="0000FF" ulstyle="single" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <u/>
+      <name val="等线"/>
+      <color rgb="FF800080"/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <u val="single"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="800080" ulstyle="single" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <u/>
+      <name val="等线"/>
+      <b/>
+      <color rgb="FF44546A"/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="44546A" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <color rgb="FFFF0000"/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="FF0000" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <b/>
+      <color rgb="FF44546A"/>
+      <sz val="18"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="44546A" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="360" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="360" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="360" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <i/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="7F7F7F" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" i="1"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" i="1"/>
+            <pm:ea face="SimSun" sz="220" lang="default" i="1"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <b/>
+      <color rgb="FF44546A"/>
+      <sz val="15"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="44546A" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="300" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="300" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="300" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color rgb="FF44546A"/>
+      <sz val="13"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="44546A" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="260" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="260" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="260" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="3F3F3F" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
       <b/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="FA7D00" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
       <b/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="FFFFFF" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="FA7D00" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <b/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="006100" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
+      <name val="等线"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="9C6500" ulstyle="none" kern="1">
+            <pm:latin face="等线" sz="220" lang="default"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default"/>
+            <pm:ea face="SimSun" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="MS Gothic"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="9.50"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1753718275" fgClr="3F3F76" bgClr="FFFF00" ulstyle="none">
+            <pm:latin face="MS Gothic" sz="190" lang="default"/>
+            <pm:cs face="Arial" sz="190" lang="default"/>
+            <pm:ea face="Arial" sz="190" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,198 +950,418 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFEBEBEB"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC7C7C7"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF4AF82"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFD964"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFE1EFD8"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFBE3D5"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF8CAAB"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFF2CA"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFE697"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC5DFB3"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA8D08C"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
+          </ext>
+        </extLst>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1753718275" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+  <borders count="38">
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
     </border>
     <border>
       <left style="thin">
@@ -966,7 +1376,73 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
     </border>
     <border>
       <left style="thin">
@@ -981,25 +1457,115 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
+            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
+            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="5B9BD5"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="ACCCEA"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
     </border>
     <border>
       <left style="thin">
@@ -1014,7 +1580,40 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+            <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
+          </pm:border>
+        </ext>
+      </extLst>
     </border>
     <border>
       <left style="double">
@@ -1029,245 +1628,867 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="left" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+            <pm:line position="right" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="FF8001"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF5B9BD5"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
+            <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1753718275"/>
+        </ext>
+      </extLst>
     </border>
   </borders>
   <cellStyleXfs count="52">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="14">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="15">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="16">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="18">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="19">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="20">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="21">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="22">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="23">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="24">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="12" xfId="25">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" xfId="26">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="14" xfId="27">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="28">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="16" xfId="29">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="30">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="31">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" xfId="32">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="33"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="20" xfId="34">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="21" xfId="35">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="22" xfId="36">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" xfId="37">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="24" xfId="38">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="25" xfId="39">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="40"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="26" xfId="41">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="27" xfId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="28" xfId="43">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="29" xfId="44">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="30" xfId="45">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="31" xfId="46">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="32" xfId="47">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="33" xfId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="34" xfId="49">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="35" xfId="50">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="36" xfId="51">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="40"/>
   </cellXfs>
   <cellStyles count="52">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="1" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="3" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="5" builtinId="6" customBuiltin="1"/>
     <cellStyle name="標準 3" xfId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="7" builtinId="39"/>
-    <cellStyle name="差" xfId="8" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="9" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="10" builtinId="40"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8"/>
-    <cellStyle name="百分比" xfId="12" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="13" builtinId="9"/>
-    <cellStyle name="注释" xfId="14" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
-    <cellStyle name="标题" xfId="18" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
-    <cellStyle name="输出" xfId="25" builtinId="21"/>
-    <cellStyle name="计算" xfId="26" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="28" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="30" builtinId="24"/>
-    <cellStyle name="汇总" xfId="31" builtinId="25"/>
-    <cellStyle name="好" xfId="32" builtinId="26"/>
+    <cellStyle name="40% - Accent3" xfId="7" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="9" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="12" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="15" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="16" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="17" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="18" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="19" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="20" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="21" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="23" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="24" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="25" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="28" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="30" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="32" builtinId="26" customBuiltin="1"/>
     <cellStyle name="標準 2 2" xfId="33"/>
-    <cellStyle name="适中" xfId="34" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="36" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="37" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="38" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="39" builtinId="34"/>
+    <cellStyle name="Neutral" xfId="34" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="36" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="37" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="38" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="39" builtinId="34" customBuiltin="1"/>
     <cellStyle name="標準 2" xfId="40"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="41" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="42" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="43" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="44" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="45" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="46" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="47" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="48" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="49" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="50" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="51" builtinId="52"/>
+    <cellStyle name="40% - Accent2" xfId="41" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="42" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="43" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="44" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="45" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="46" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="47" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="49" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="50" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="51" builtinId="52" customBuiltin="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="smNativeData">
+      <pm:charStyles xmlns:pm="smNativeData" id="1753718275" count="1">
+        <pm:charStyle name="標準" fontId="0" Id="1"/>
+      </pm:charStyles>
+      <pm:colors xmlns:pm="smNativeData" id="1753718275" count="42">
+        <pm:color name="色 24" rgb="3F3F76"/>
+        <pm:color name="色 25" rgb="9C0006"/>
+        <pm:color name="色 26" rgb="800080"/>
+        <pm:color name="色 27" rgb="44546A"/>
+        <pm:color name="色 28" rgb="3F3F3F"/>
+        <pm:color name="色 29" rgb="FA7D00"/>
+        <pm:color name="色 30" rgb="006100"/>
+        <pm:color name="色 31" rgb="9C6500"/>
+        <pm:color name="色 32" rgb="EBEBEB"/>
+        <pm:color name="*20%灰色" rgb="000000"/>
+        <pm:color name="色 34" rgb="FFCC99"/>
+        <pm:color name="色 35" rgb="D9D9D9"/>
+        <pm:color name="色 36" rgb="FFC7CE"/>
+        <pm:color name="色 37" rgb="C7C7C7"/>
+        <pm:color name="色 38" rgb="FFFFCC"/>
+        <pm:color name="色 39" rgb="F4AF82"/>
+        <pm:color name="色 40" rgb="9BC2E6"/>
+        <pm:color name="色 41" rgb="FFD964"/>
+        <pm:color name="色 42" rgb="F2F2F2"/>
+        <pm:color name="色 43" rgb="A5A5A5"/>
+        <pm:color name="色 44" rgb="E1EFD8"/>
+        <pm:color name="色 45" rgb="ED7D31"/>
+        <pm:color name="色 46" rgb="C6EFCE"/>
+        <pm:color name="色 47" rgb="FFEB9C"/>
+        <pm:color name="色 48" rgb="D9E1F2"/>
+        <pm:color name="色 49" rgb="5B9BD5"/>
+        <pm:color name="色 50" rgb="DDEBF7"/>
+        <pm:color name="色 51" rgb="BDD7EE"/>
+        <pm:color name="色 52" rgb="FBE3D5"/>
+        <pm:color name="色 53" rgb="F8CAAB"/>
+        <pm:color name="色 54" rgb="FFC000"/>
+        <pm:color name="色 55" rgb="FFF2CA"/>
+        <pm:color name="色 56" rgb="FFE697"/>
+        <pm:color name="色 57" rgb="4472C4"/>
+        <pm:color name="色 58" rgb="B4C6E7"/>
+        <pm:color name="色 59" rgb="8EA9DB"/>
+        <pm:color name="色 60" rgb="70AD47"/>
+        <pm:color name="色 61" rgb="C5DFB3"/>
+        <pm:color name="色 62" rgb="A8D08C"/>
+        <pm:color name="色 63" rgb="B2B2B2"/>
+        <pm:color name="色 64" rgb="ACCCEA"/>
+        <pm:color name="色 65" rgb="FF8001"/>
+      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
@@ -1284,106 +2505,46 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="EEECE1"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="1F497D"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="等线"/>
+        <a:ea typeface="SimSun"/>
+        <a:cs typeface="Times New Roman"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1395,156 +2556,214 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr>
+        <a:prstTxWarp prst="textNoShape">
+          <a:avLst/>
+        </a:prstTxWarp>
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr>
+          <a:defRPr/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView view="normal" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85"/>
+  <sheetFormatPr defaultRowHeight="14.60"/>
   <cols>
-    <col min="1" max="1" width="22.7522123893805" customWidth="1"/>
-    <col min="2" max="2" width="62.2477876106195" customWidth="1"/>
-    <col min="3" max="12" width="4.6283185840708" customWidth="1"/>
-    <col min="13" max="13" width="74" customWidth="1"/>
-    <col min="14" max="14" width="4.75221238938053" customWidth="1"/>
-    <col min="15" max="15" width="22.3716814159292" customWidth="1"/>
+    <col min="1" max="1" width="22.754098" customWidth="1"/>
+    <col min="2" max="2" width="62.245902" customWidth="1"/>
+    <col min="3" max="12" width="4.631148" customWidth="1"/>
+    <col min="13" max="13" width="74.000000" customWidth="1"/>
+    <col min="14" max="14" width="4.754098" customWidth="1"/>
+    <col min="15" max="15" width="22.368852" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
@@ -1607,7 +2826,7 @@
       <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="40" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1621,7 +2840,7 @@
       <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="40" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1635,7 +2854,7 @@
       <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="40" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1649,7 +2868,7 @@
       <c r="M5" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="40" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1663,7 +2882,7 @@
       <c r="M6" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="40" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1677,7 +2896,7 @@
       <c r="M8" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="40" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1724,27 +2943,50 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1753718275" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1753718275" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1753718275" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1753718275" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1753718275" Id="1" type="0" value="0"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1753718275" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85"/>
+  <sheetFormatPr defaultRowHeight="14.60"/>
   <cols>
-    <col min="1" max="1" width="38.3716814159292" customWidth="1"/>
-    <col min="2" max="2" width="15.2477876106195" customWidth="1"/>
-    <col min="3" max="12" width="3.6283185840708" customWidth="1"/>
-    <col min="13" max="13" width="56.2477876106195" customWidth="1"/>
+    <col min="1" max="1" width="38.368852" customWidth="1"/>
+    <col min="2" max="2" width="15.245902" customWidth="1"/>
+    <col min="3" max="12" width="3.631148" customWidth="1"/>
+    <col min="13" max="13" width="56.245902" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
@@ -1807,7 +3049,7 @@
       <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1821,7 +3063,7 @@
       <c r="M3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="6" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1835,7 +3077,7 @@
       <c r="M4" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1849,7 +3091,7 @@
       <c r="M5" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1863,7 +3105,7 @@
       <c r="M6" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1877,7 +3119,7 @@
       <c r="M7" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="6" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1891,7 +3133,7 @@
       <c r="M8" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1905,7 +3147,7 @@
       <c r="M9" t="s">
         <v>82</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1919,7 +3161,7 @@
       <c r="M10" t="s">
         <v>86</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1933,7 +3175,7 @@
       <c r="M11" t="s">
         <v>90</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="6" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1947,7 +3189,7 @@
       <c r="M12" t="s">
         <v>94</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1961,7 +3203,7 @@
       <c r="M13" t="s">
         <v>98</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="6" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1975,7 +3217,7 @@
       <c r="M14" t="s">
         <v>102</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" s="6" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1989,7 +3231,7 @@
       <c r="M15" t="s">
         <v>106</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="6" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2003,7 +3245,7 @@
       <c r="M16" t="s">
         <v>110</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="6" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2017,7 +3259,7 @@
       <c r="M17" t="s">
         <v>114</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2031,7 +3273,7 @@
       <c r="M18" t="s">
         <v>118</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2045,7 +3287,7 @@
       <c r="M19" t="s">
         <v>122</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="6" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2059,7 +3301,7 @@
       <c r="M20" t="s">
         <v>126</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2073,7 +3315,7 @@
       <c r="M21" t="s">
         <v>130</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="6" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2105,7 +3347,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" ht="21" customHeight="1" spans="1:15">
+    <row r="24" spans="1:15" ht="21" customHeight="1">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -2147,7 +3389,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" ht="20.25" customHeight="1" spans="1:15">
+    <row r="27" spans="1:15" ht="20.25" customHeight="1">
       <c r="A27" t="s">
         <v>152</v>
       </c>
@@ -2189,7 +3431,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" ht="18.75" customHeight="1" spans="1:15">
+    <row r="30" spans="1:15" ht="18.75" customHeight="1">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -2273,36 +3515,92 @@
         <v>187</v>
       </c>
     </row>
-    <row r="51" ht="18" customHeight="1"/>
-    <row r="52" ht="20.25" customHeight="1"/>
-    <row r="53" ht="19.5" customHeight="1"/>
-    <row r="54" ht="18.75" customHeight="1"/>
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
+        <v>188</v>
+      </c>
+      <c r="M36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="M37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" t="s">
+        <v>192</v>
+      </c>
+      <c r="M38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="M39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" customHeight="1"/>
+    <row r="52" spans="1:1" ht="20.25" customHeight="1"/>
+    <row r="53" spans="1:1" ht="19.50" customHeight="1"/>
+    <row r="54" spans="1:1" ht="18.75" customHeight="1"/>
     <row r="55" spans="13:13">
-      <c r="M55" s="2"/>
+      <c r="M55" s="52"/>
     </row>
     <row r="56" spans="13:13">
-      <c r="M56" s="2"/>
-    </row>
-    <row r="57" ht="39" customHeight="1" spans="13:13">
-      <c r="M57" s="2"/>
+      <c r="M56" s="52"/>
+    </row>
+    <row r="57" spans="13:13" ht="39" customHeight="1">
+      <c r="M57" s="52"/>
     </row>
     <row r="58" spans="13:13">
-      <c r="M58" s="2"/>
+      <c r="M58" s="52"/>
     </row>
     <row r="60" spans="13:13">
-      <c r="M60" s="2"/>
-    </row>
-    <row r="74" ht="18.75" customHeight="1"/>
-    <row r="75" ht="20.25" customHeight="1"/>
+      <c r="M60" s="52"/>
+    </row>
+    <row r="74" spans="1:1" ht="18.75" customHeight="1"/>
+    <row r="75" spans="1:1" ht="20.25" customHeight="1"/>
     <row r="79" spans="13:13">
-      <c r="M79" s="2"/>
+      <c r="M79" s="52"/>
     </row>
     <row r="80" spans="13:13">
-      <c r="M80" s="2"/>
+      <c r="M80" s="52"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1753718275" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1753718275" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1753718275" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1753718275" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1753718275" Id="1" type="0" value="0"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1753718275" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>